<commit_message>
electricity for vehicles, PV, areas and fuels for industry
</commit_message>
<xml_diff>
--- a/Data/The Three Scenarios.xlsx
+++ b/Data/The Three Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORHEN\Desktop\Research-Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DORHEN\Desktop\Shared-Project\NewVersion\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B9E8B8-4C43-4918-A163-9C547DE7A5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CAA40C-90EF-4A2A-863D-C102D59A3048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -104,12 +104,6 @@
     <t>s3</t>
   </si>
   <si>
-    <t>change in electricity consumption per capita in 2030</t>
-  </si>
-  <si>
-    <t>Change in desalinated water in 2030</t>
-  </si>
-  <si>
     <t>reducing beef consumption</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>electricity saving</t>
   </si>
   <si>
-    <t>waste minimization</t>
-  </si>
-  <si>
     <t>burning waste</t>
   </si>
   <si>
@@ -176,9 +167,6 @@
     <t xml:space="preserve"> electric truck vehicle</t>
   </si>
   <si>
-    <t xml:space="preserve">population growth by 2030 </t>
-  </si>
-  <si>
     <t>Electricity</t>
   </si>
   <si>
@@ -450,6 +438,18 @@
   </si>
   <si>
     <t>Advanced</t>
+  </si>
+  <si>
+    <t>population growth</t>
+  </si>
+  <si>
+    <t>change in electricity consumption per capita</t>
+  </si>
+  <si>
+    <t>Change in desalinated water</t>
+  </si>
+  <si>
+    <t>fuel for energy</t>
   </si>
 </sst>
 </file>
@@ -1251,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1275,27 +1275,27 @@
         <v>2</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
       <c r="B2" s="4">
         <v>0</v>
@@ -1322,12 +1322,12 @@
         <v>0.9</v>
       </c>
       <c r="J2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>116</v>
       </c>
       <c r="B3" s="4">
         <v>0</v>
@@ -1354,12 +1354,12 @@
         <v>0.41</v>
       </c>
       <c r="J3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>117</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -1386,12 +1386,12 @@
         <v>2.64</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -1418,12 +1418,12 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="17">
         <v>0</v>
@@ -1450,12 +1450,12 @@
         <v>0.08</v>
       </c>
       <c r="J6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>0.1</v>
@@ -1482,12 +1482,12 @@
         <v>0.8</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9">
         <v>0.63100000000000001</v>
@@ -1514,12 +1514,12 @@
         <v>0.2</v>
       </c>
       <c r="J8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="4">
         <v>0.2</v>
@@ -1546,12 +1546,12 @@
         <v>0.16</v>
       </c>
       <c r="J9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="5">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E10" s="16">
         <v>0</v>
@@ -1572,19 +1572,19 @@
         <v>0</v>
       </c>
       <c r="H10" s="19">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I10" s="19">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="J10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="K10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B11" s="4">
         <v>0.51</v>
@@ -1611,12 +1611,12 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="4">
         <v>0.26</v>
@@ -1643,12 +1643,12 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
@@ -1675,12 +1675,12 @@
         <v>0.3</v>
       </c>
       <c r="J13" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="4">
         <v>0.04</v>
@@ -1707,12 +1707,12 @@
         <v>0.5</v>
       </c>
       <c r="J14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="4">
         <v>0</v>
@@ -1739,12 +1739,12 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4">
         <v>0</v>
@@ -1771,12 +1771,12 @@
         <v>0.3</v>
       </c>
       <c r="J16" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4">
         <v>0</v>
@@ -1803,12 +1803,12 @@
         <v>0.25</v>
       </c>
       <c r="J17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" s="4">
         <v>0</v>
@@ -1835,12 +1835,12 @@
         <v>1</v>
       </c>
       <c r="J18" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B19" s="4">
         <v>0.75</v>
@@ -1867,12 +1867,12 @@
         <v>0</v>
       </c>
       <c r="J19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B20" s="4">
         <v>0.05</v>
@@ -1899,7 +1899,7 @@
         <v>0.1</v>
       </c>
       <c r="J20" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1912,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1924,13 +1924,13 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2" s="23">
         <v>0</v>
@@ -1938,15 +1938,15 @@
     </row>
     <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3" s="23">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B4" s="23">
         <v>0.5</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B5" s="25">
         <v>0</v>
@@ -1986,388 +1986,388 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B1" s="37"/>
       <c r="D1" s="37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6" s="31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" s="37"/>
       <c r="D7" s="32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A14" s="37" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B14" s="37"/>
       <c r="D14" s="34" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="29" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D22" s="33" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D23" s="33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" s="33" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D25" s="33" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D26" s="33" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D27" s="33" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D28" s="33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D29" s="33" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D30" s="33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D31" s="33" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D32" s="33" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" s="33" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" s="33" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" s="33" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D36" s="33" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D37" s="33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D38" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D39" s="33" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D40" s="33" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D41" s="33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D42" s="33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D43" s="33" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D44" s="33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D45" s="33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="46" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D46" s="33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="47" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D47" s="33" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D48" s="33" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D49" s="33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D50" s="33" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D51" s="33" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D52" s="33" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D53" s="33" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D54" s="33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D55" s="33" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D56" s="33" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="57" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D57" s="33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D58" s="33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D59" s="33" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="60" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D60" s="33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="61" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D61" s="33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D62" s="33" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D63" s="33" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D64" s="33" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D65" s="33" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>